<commit_message>
Commit kmk007 update print report
</commit_message>
<xml_diff>
--- a/nts.uk/uk.at/at.file/nts.uk.file.at.infra/src/main/resources/report/kmk007.xlsx
+++ b/nts.uk/uk.at/at.file/nts.uk.file.at.infra/src/main/resources/report/kmk007.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="22155" windowHeight="11535"/>
   </bookViews>
   <sheets>
-    <sheet name="出力イメージ" sheetId="1" r:id="rId1"/>
+    <sheet name="ﾏｽﾀﾘｽﾄ" sheetId="1" r:id="rId1"/>
   </sheets>
   <externalReferences>
     <externalReference r:id="rId2"/>
@@ -160,7 +160,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
   <si>
     <t>略名</t>
     <rPh sb="0" eb="1">
@@ -306,33 +306,9 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>001</t>
-  </si>
-  <si>
-    <t>出勤</t>
-    <rPh sb="0" eb="2">
-      <t>シュッキン</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>名称</t>
     <rPh sb="0" eb="2">
       <t>メイショウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>出</t>
-    <rPh sb="0" eb="1">
-      <t>シュツ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>1日</t>
-    <rPh sb="1" eb="2">
-      <t>ニチ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -360,30 +336,12 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>出勤です</t>
-    <rPh sb="0" eb="2">
-      <t>シュッキン</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>対象範囲</t>
     <rPh sb="0" eb="2">
       <t>タイショウ</t>
     </rPh>
     <rPh sb="2" eb="4">
       <t>ハンイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Swork</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>出勤とする</t>
-    <rPh sb="0" eb="2">
-      <t>シュッキン</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -410,25 +368,6 @@
     <rPh sb="0" eb="2">
       <t>ゴゴ</t>
     </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>出勤</t>
-    <rPh sb="0" eb="2">
-      <t>シュッキン</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>ー</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>○</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>○</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -497,7 +436,91 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>StandardWork</t>
+    <t>&amp;=list.workTypeCode</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>&amp;=list.name</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>&amp;=list.symbolicName</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>&amp;=list.abbreviationName</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>&amp;=list.memo</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>&amp;=list.deprecate</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>&amp;=list.calculateMethod</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>&amp;=list.workAtr</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>&amp;=list.oneDayCls</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>&amp;=list.morningCls</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>&amp;=list.afternoonCls</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>&amp;=list.dayNightTimeAsk</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>&amp;=list.attendanceTime</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>&amp;=list.timeLeaveWork</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>&amp;=list.timeLeaveWork</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>&amp;=list.digestPublicHd</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>&amp;=list.genSubHodiday</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>&amp;=list.sumAbsenseNo</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>&amp;=list.sumSpHodidayNo</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>&amp;=list.closeAtr</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>&amp;=list.otherLangName</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>&amp;=list.otherLangShortName</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -505,7 +528,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -532,6 +555,15 @@
       <name val="Meiryo UI"/>
       <family val="2"/>
       <charset val="128"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -579,7 +611,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -602,6 +634,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -44213,10 +44249,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:V10"/>
+  <dimension ref="A3:V17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="V9" sqref="V9"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="13.5"/>
@@ -44230,34 +44266,34 @@
   <sheetData>
     <row r="3" spans="1:22">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:22">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:22">
       <c r="A5" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:22">
       <c r="A6" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="B6" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:22">
@@ -44270,10 +44306,10 @@
     </row>
     <row r="9" spans="1:22" s="8" customFormat="1">
       <c r="A9" s="3" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>0</v>
@@ -44285,22 +44321,22 @@
         <v>2</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="G9" s="3" t="s">
         <v>8</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="L9" s="3" t="s">
         <v>3</v>
@@ -44327,80 +44363,88 @@
         <v>11</v>
       </c>
       <c r="T9" s="3" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="U9" s="3" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="V9" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:22" s="8" customFormat="1">
       <c r="A10" s="3" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
-      <c r="F10" s="5"/>
+      <c r="F10" s="5" t="s">
+        <v>35</v>
+      </c>
       <c r="G10" s="3" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>16</v>
+        <v>37</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="L10" s="7" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="M10" s="7" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="N10" s="7" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="O10" s="7" t="s">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="P10" s="7" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="Q10" s="7" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="R10" s="7" t="s">
-        <v>28</v>
+        <v>47</v>
       </c>
       <c r="S10" s="7" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="T10" s="7" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="U10" s="3" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="V10" s="3" t="s">
-        <v>21</v>
+        <v>51</v>
       </c>
+    </row>
+    <row r="14" spans="1:22">
+      <c r="O14" s="9"/>
+    </row>
+    <row r="17" spans="7:7">
+      <c r="G17" s="10"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>

</xml_diff>